<commit_message>
updating UI for multiple segments
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/verbatim_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/verbatim_NUEDEXTA-2test.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="T1 - Test Topic" sheetId="1" r:id="rId4"/>
-    <sheet name="T2 - Test2" sheetId="2" r:id="rId5"/>
+    <sheet name="T1 - TEst" sheetId="1" r:id="rId4"/>
+    <sheet name="T2 - Test 2" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -172,9 +172,9 @@
     <tableColumn id="3" name="Why"/>
     <tableColumn id="4" name="S"/>
     <tableColumn id="5" name="Valence"/>
-    <tableColumn id="6" name="Mindset"/>
+    <tableColumn id="6" name="Test"/>
     <tableColumn id="7" name="Segment"/>
-    <tableColumn id="8" name="Product Mindset"/>
+    <tableColumn id="8" name="test 2"/>
     <tableColumn id="9" name="Response ID"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0" name="TableStyleMedium9"/>
@@ -190,9 +190,9 @@
     <tableColumn id="3" name="Why"/>
     <tableColumn id="4" name="S"/>
     <tableColumn id="5" name="Valence"/>
-    <tableColumn id="6" name="Mindset"/>
+    <tableColumn id="6" name="Test"/>
     <tableColumn id="7" name="Segment"/>
-    <tableColumn id="8" name="Product Mindset"/>
+    <tableColumn id="8" name="test 2"/>
     <tableColumn id="9" name="Response ID"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0" name="TableStyleMedium9"/>
@@ -224,14 +224,14 @@
     <row r="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Test Topic</t>
+          <t>TEst</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Fram</t>
+          <t>Test Frame</t>
         </is>
       </c>
     </row>
@@ -263,7 +263,7 @@
       </c>
       <c r="F3" s="6" t="inlineStr">
         <is>
-          <t>Mindset</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="G3" s="6" t="inlineStr">
@@ -273,7 +273,7 @@
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>Product Mindset</t>
+          <t>test 2</t>
         </is>
       </c>
       <c r="I3" s="6" t="inlineStr">
@@ -306,7 +306,7 @@
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
@@ -349,7 +349,7 @@
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -392,7 +392,7 @@
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
@@ -435,7 +435,7 @@
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G9" s="4" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G10" s="4" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G11" s="4" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G12" s="4" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G15" s="4" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G16" s="4" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G17" s="4" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G18" s="4" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="F19" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G19" s="4" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G21" s="4" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G22" s="4" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G23" s="4" t="inlineStr">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="F25" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G25" s="4" t="inlineStr">
@@ -1252,7 +1252,7 @@
       </c>
       <c r="F26" s="4" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G26" s="4" t="inlineStr">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="F28" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G28" s="4" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="F29" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G29" s="4" t="inlineStr">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="F31" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G31" s="4" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G32" s="4" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="F33" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G33" s="4" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="F34" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G34" s="4" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F36" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G36" s="4" t="inlineStr">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F37" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G37" s="4" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G38" s="4" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="F39" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G39" s="4" t="inlineStr">
@@ -1854,7 +1854,7 @@
       </c>
       <c r="F40" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G40" s="4" t="inlineStr">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="F41" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G41" s="4" t="inlineStr">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="F42" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G42" s="4" t="inlineStr">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="F43" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G43" s="4" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="F44" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G44" s="4" t="inlineStr">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="F46" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G46" s="4" t="inlineStr">
@@ -2155,7 +2155,7 @@
       </c>
       <c r="F47" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G47" s="4" t="inlineStr">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="F48" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G48" s="4" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="F49" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G49" s="4" t="inlineStr">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="F50" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G50" s="4" t="inlineStr">
@@ -2327,7 +2327,7 @@
       </c>
       <c r="F51" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G51" s="4" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="F52" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G52" s="4" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="F53" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G53" s="4" t="inlineStr">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="F54" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G54" s="4" t="inlineStr">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="F55" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G55" s="4" t="inlineStr">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="F56" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G56" s="4" t="inlineStr">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="F57" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G57" s="4" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G58" s="4" t="inlineStr">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="F59" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G59" s="4" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="F60" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G60" s="4" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="F61" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G61" s="4" t="inlineStr">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G62" s="4" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F63" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G63" s="4" t="inlineStr">
@@ -2886,7 +2886,7 @@
       </c>
       <c r="F64" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G64" s="4" t="inlineStr">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="F65" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G65" s="4" t="inlineStr">
@@ -2972,7 +2972,7 @@
       </c>
       <c r="F66" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G66" s="4" t="inlineStr">
@@ -3015,7 +3015,7 @@
       </c>
       <c r="F67" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G67" s="4" t="inlineStr">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="F68" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G68" s="4" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="F69" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G69" s="4" t="inlineStr">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="F70" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G70" s="4" t="inlineStr">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="F72" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G72" s="4" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="F73" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G73" s="4" t="inlineStr">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="F74" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G74" s="4" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="F75" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G75" s="4" t="inlineStr">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="F76" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G76" s="4" t="inlineStr">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="F79" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G79" s="4" t="inlineStr">
@@ -3574,7 +3574,7 @@
       </c>
       <c r="F80" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G80" s="4" t="inlineStr">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="F81" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G81" s="4" t="inlineStr">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="F82" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G82" s="4" t="inlineStr">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="F83" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G83" s="4" t="inlineStr">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="F84" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G84" s="4" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="F85" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G85" s="4" t="inlineStr">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="F86" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G86" s="4" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="F87" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G87" s="4" t="inlineStr">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="F88" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G88" s="4" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="F89" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G89" s="4" t="inlineStr">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="F90" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G90" s="4" t="inlineStr">
@@ -4047,7 +4047,7 @@
       </c>
       <c r="F91" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G91" s="4" t="inlineStr">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="F92" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G92" s="4" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="F93" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G93" s="4" t="inlineStr">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="F94" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G94" s="4" t="inlineStr">
@@ -4219,7 +4219,7 @@
       </c>
       <c r="F95" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G95" s="4" t="inlineStr">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="F96" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G96" s="4" t="inlineStr">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="F97" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G97" s="4" t="inlineStr">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="F98" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G98" s="4" t="inlineStr">
@@ -4391,7 +4391,7 @@
       </c>
       <c r="F99" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G99" s="4" t="inlineStr">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="F100" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G100" s="4" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="F101" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G101" s="4" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="F102" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G102" s="4" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="F103" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G103" s="4" t="inlineStr">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="F104" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G104" s="4" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="F105" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G105" s="4" t="inlineStr">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="F106" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G106" s="4" t="inlineStr">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="F108" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G108" s="4" t="inlineStr">
@@ -4821,7 +4821,7 @@
       </c>
       <c r="F109" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G109" s="4" t="inlineStr">
@@ -4864,7 +4864,7 @@
       </c>
       <c r="F110" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G110" s="4" t="inlineStr">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="F111" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G111" s="4" t="inlineStr">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="F112" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G112" s="4" t="inlineStr">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="F115" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G115" s="4" t="inlineStr">
@@ -5122,7 +5122,7 @@
       </c>
       <c r="F116" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G116" s="4" t="inlineStr">
@@ -5165,7 +5165,7 @@
       </c>
       <c r="F117" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G117" s="4" t="inlineStr">
@@ -5208,7 +5208,7 @@
       </c>
       <c r="F118" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G118" s="4" t="inlineStr">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="F119" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G119" s="4" t="inlineStr">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="F120" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G120" s="4" t="inlineStr">
@@ -5337,7 +5337,7 @@
       </c>
       <c r="F121" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G121" s="4" t="inlineStr">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="F122" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G122" s="4" t="inlineStr">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="F123" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G123" s="4" t="inlineStr">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="F124" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G124" s="4" t="inlineStr">
@@ -5509,7 +5509,7 @@
       </c>
       <c r="F125" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G125" s="4" t="inlineStr">
@@ -5552,7 +5552,7 @@
       </c>
       <c r="F126" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G126" s="4" t="inlineStr">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="F127" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G127" s="4" t="inlineStr">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="F128" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G128" s="4" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="F129" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G129" s="4" t="inlineStr">
@@ -5724,7 +5724,7 @@
       </c>
       <c r="F130" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G130" s="4" t="inlineStr">
@@ -5767,7 +5767,7 @@
       </c>
       <c r="F131" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G131" s="4" t="inlineStr">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="F132" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G132" s="4" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="F133" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G133" s="4" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="F134" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G134" s="4" t="inlineStr">
@@ -5939,7 +5939,7 @@
       </c>
       <c r="F135" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G135" s="4" t="inlineStr">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="F136" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G136" s="4" t="inlineStr">
@@ -6025,7 +6025,7 @@
       </c>
       <c r="F137" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G137" s="4" t="inlineStr">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="F138" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G138" s="4" t="inlineStr">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="F139" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G139" s="4" t="inlineStr">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="F140" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G140" s="4" t="inlineStr">
@@ -6197,7 +6197,7 @@
       </c>
       <c r="F141" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G141" s="4" t="inlineStr">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="F142" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G142" s="4" t="inlineStr">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="F143" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G143" s="4" t="inlineStr">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="F144" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G144" s="4" t="inlineStr">
@@ -6369,7 +6369,7 @@
       </c>
       <c r="F145" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G145" s="4" t="inlineStr">
@@ -6412,7 +6412,7 @@
       </c>
       <c r="F146" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G146" s="4" t="inlineStr">
@@ -6455,7 +6455,7 @@
       </c>
       <c r="F147" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G147" s="4" t="inlineStr">
@@ -6498,7 +6498,7 @@
       </c>
       <c r="F148" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G148" s="4" t="inlineStr">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="F149" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G149" s="4" t="inlineStr">
@@ -6584,7 +6584,7 @@
       </c>
       <c r="F150" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G150" s="4" t="inlineStr">
@@ -6627,7 +6627,7 @@
       </c>
       <c r="F151" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G151" s="4" t="inlineStr">
@@ -6670,7 +6670,7 @@
       </c>
       <c r="F152" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G152" s="4" t="inlineStr">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="F153" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G153" s="4" t="inlineStr">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="F154" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G154" s="4" t="inlineStr">
@@ -6799,7 +6799,7 @@
       </c>
       <c r="F155" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G155" s="4" t="inlineStr">
@@ -6842,7 +6842,7 @@
       </c>
       <c r="F156" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G156" s="4" t="inlineStr">
@@ -6885,7 +6885,7 @@
       </c>
       <c r="F157" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G157" s="4" t="inlineStr">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="F158" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G158" s="4" t="inlineStr">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="F159" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G159" s="4" t="inlineStr">
@@ -7014,7 +7014,7 @@
       </c>
       <c r="F160" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G160" s="4" t="inlineStr">
@@ -7057,7 +7057,7 @@
       </c>
       <c r="F161" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G161" s="4" t="inlineStr">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="F162" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G162" s="4" t="inlineStr">
@@ -7143,7 +7143,7 @@
       </c>
       <c r="F163" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G163" s="4" t="inlineStr">
@@ -7186,7 +7186,7 @@
       </c>
       <c r="F164" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G164" s="4" t="inlineStr">
@@ -7229,7 +7229,7 @@
       </c>
       <c r="F165" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G165" s="4" t="inlineStr">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="F166" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G166" s="4" t="inlineStr">
@@ -7315,7 +7315,7 @@
       </c>
       <c r="F167" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G167" s="4" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="F168" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G168" s="4" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="F169" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G169" s="4" t="inlineStr">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="F170" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G170" s="4" t="inlineStr">
@@ -7487,7 +7487,7 @@
       </c>
       <c r="F171" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G171" s="4" t="inlineStr">
@@ -7530,7 +7530,7 @@
       </c>
       <c r="F172" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G172" s="4" t="inlineStr">
@@ -7573,7 +7573,7 @@
       </c>
       <c r="F173" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G173" s="4" t="inlineStr">
@@ -7616,7 +7616,7 @@
       </c>
       <c r="F174" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G174" s="4" t="inlineStr">
@@ -7659,7 +7659,7 @@
       </c>
       <c r="F175" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G175" s="4" t="inlineStr">
@@ -7702,7 +7702,7 @@
       </c>
       <c r="F176" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G176" s="4" t="inlineStr">
@@ -7745,7 +7745,7 @@
       </c>
       <c r="F177" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G177" s="4" t="inlineStr">
@@ -7788,7 +7788,7 @@
       </c>
       <c r="F178" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G178" s="4" t="inlineStr">
@@ -7831,7 +7831,7 @@
       </c>
       <c r="F179" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G179" s="4" t="inlineStr">
@@ -7874,7 +7874,7 @@
       </c>
       <c r="F180" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G180" s="4" t="inlineStr">
@@ -7917,7 +7917,7 @@
       </c>
       <c r="F181" s="4" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G181" s="4" t="inlineStr">
@@ -7960,7 +7960,7 @@
       </c>
       <c r="F182" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G182" s="4" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="F183" s="4" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G183" s="4" t="inlineStr">
@@ -8063,14 +8063,14 @@
     <row r="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
-          <t>Test2</t>
+          <t>Test 2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Frame of Reference</t>
+          <t>Test Frame 2</t>
         </is>
       </c>
     </row>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="F3" s="10" t="inlineStr">
         <is>
-          <t>Mindset</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="G3" s="10" t="inlineStr">
@@ -8112,7 +8112,7 @@
       </c>
       <c r="H3" s="10" t="inlineStr">
         <is>
-          <t>Product Mindset</t>
+          <t>test 2</t>
         </is>
       </c>
       <c r="I3" s="10" t="inlineStr">
@@ -8145,7 +8145,7 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
@@ -8188,7 +8188,7 @@
       </c>
       <c r="F5" s="8" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G5" s="8" t="inlineStr">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="F6" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G6" s="8" t="inlineStr">
@@ -8274,7 +8274,7 @@
       </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
-          <t>Impassioned</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G7" s="8" t="inlineStr">
@@ -8532,7 +8532,7 @@
       </c>
       <c r="F13" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G13" s="8" t="inlineStr">
@@ -8618,7 +8618,7 @@
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G15" s="8" t="inlineStr">
@@ -8704,7 +8704,7 @@
       </c>
       <c r="F17" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G17" s="8" t="inlineStr">
@@ -8790,7 +8790,7 @@
       </c>
       <c r="F19" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G19" s="8" t="inlineStr">
@@ -8833,7 +8833,7 @@
       </c>
       <c r="F20" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G20" s="8" t="inlineStr">
@@ -9091,7 +9091,7 @@
       </c>
       <c r="F26" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G26" s="8" t="inlineStr">
@@ -9134,7 +9134,7 @@
       </c>
       <c r="F27" s="8" t="inlineStr">
         <is>
-          <t>Attracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G27" s="8" t="inlineStr">
@@ -9177,7 +9177,7 @@
       </c>
       <c r="F28" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G28" s="8" t="inlineStr">
@@ -9220,7 +9220,7 @@
       </c>
       <c r="F29" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G29" s="8" t="inlineStr">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="F30" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G30" s="8" t="inlineStr">
@@ -9306,7 +9306,7 @@
       </c>
       <c r="F31" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G31" s="8" t="inlineStr">
@@ -9349,7 +9349,7 @@
       </c>
       <c r="F32" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G32" s="8" t="inlineStr">
@@ -9392,7 +9392,7 @@
       </c>
       <c r="F33" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G33" s="8" t="inlineStr">
@@ -9521,7 +9521,7 @@
       </c>
       <c r="F36" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G36" s="8" t="inlineStr">
@@ -9564,7 +9564,7 @@
       </c>
       <c r="F37" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G37" s="8" t="inlineStr">
@@ -9607,7 +9607,7 @@
       </c>
       <c r="F38" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G38" s="8" t="inlineStr">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="F39" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G39" s="8" t="inlineStr">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="F40" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G40" s="8" t="inlineStr">
@@ -9736,7 +9736,7 @@
       </c>
       <c r="F41" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G41" s="8" t="inlineStr">
@@ -9779,7 +9779,7 @@
       </c>
       <c r="F42" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G42" s="8" t="inlineStr">
@@ -9822,7 +9822,7 @@
       </c>
       <c r="F43" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G43" s="8" t="inlineStr">
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F44" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G44" s="8" t="inlineStr">
@@ -9908,7 +9908,7 @@
       </c>
       <c r="F45" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G45" s="8" t="inlineStr">
@@ -9951,7 +9951,7 @@
       </c>
       <c r="F46" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G46" s="8" t="inlineStr">
@@ -9994,7 +9994,7 @@
       </c>
       <c r="F47" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G47" s="8" t="inlineStr">
@@ -10037,7 +10037,7 @@
       </c>
       <c r="F48" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G48" s="8" t="inlineStr">
@@ -10080,7 +10080,7 @@
       </c>
       <c r="F49" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G49" s="8" t="inlineStr">
@@ -10123,7 +10123,7 @@
       </c>
       <c r="F50" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G50" s="8" t="inlineStr">
@@ -10166,7 +10166,7 @@
       </c>
       <c r="F51" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G51" s="8" t="inlineStr">
@@ -10209,7 +10209,7 @@
       </c>
       <c r="F52" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G52" s="8" t="inlineStr">
@@ -10252,7 +10252,7 @@
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G53" s="8" t="inlineStr">
@@ -10295,7 +10295,7 @@
       </c>
       <c r="F54" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G54" s="8" t="inlineStr">
@@ -10338,7 +10338,7 @@
       </c>
       <c r="F55" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G55" s="8" t="inlineStr">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="F56" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G56" s="8" t="inlineStr">
@@ -10424,7 +10424,7 @@
       </c>
       <c r="F57" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G57" s="8" t="inlineStr">
@@ -10467,7 +10467,7 @@
       </c>
       <c r="F58" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G58" s="8" t="inlineStr">
@@ -10510,7 +10510,7 @@
       </c>
       <c r="F59" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G59" s="8" t="inlineStr">
@@ -10553,7 +10553,7 @@
       </c>
       <c r="F60" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G60" s="8" t="inlineStr">
@@ -10596,7 +10596,7 @@
       </c>
       <c r="F61" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G61" s="8" t="inlineStr">
@@ -10639,7 +10639,7 @@
       </c>
       <c r="F62" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G62" s="8" t="inlineStr">
@@ -10682,7 +10682,7 @@
       </c>
       <c r="F63" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G63" s="8" t="inlineStr">
@@ -10725,7 +10725,7 @@
       </c>
       <c r="F64" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G64" s="8" t="inlineStr">
@@ -10768,7 +10768,7 @@
       </c>
       <c r="F65" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G65" s="8" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="F66" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G66" s="8" t="inlineStr">
@@ -10854,7 +10854,7 @@
       </c>
       <c r="F67" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G67" s="8" t="inlineStr">
@@ -10897,7 +10897,7 @@
       </c>
       <c r="F68" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G68" s="8" t="inlineStr">
@@ -10940,7 +10940,7 @@
       </c>
       <c r="F69" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G69" s="8" t="inlineStr">
@@ -10983,7 +10983,7 @@
       </c>
       <c r="F70" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G70" s="8" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="F71" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G71" s="8" t="inlineStr">
@@ -11069,7 +11069,7 @@
       </c>
       <c r="F72" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G72" s="8" t="inlineStr">
@@ -11112,7 +11112,7 @@
       </c>
       <c r="F73" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G73" s="8" t="inlineStr">
@@ -11155,7 +11155,7 @@
       </c>
       <c r="F74" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G74" s="8" t="inlineStr">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="F75" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G75" s="8" t="inlineStr">
@@ -11241,7 +11241,7 @@
       </c>
       <c r="F76" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G76" s="8" t="inlineStr">
@@ -11284,7 +11284,7 @@
       </c>
       <c r="F77" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G77" s="8" t="inlineStr">
@@ -11327,7 +11327,7 @@
       </c>
       <c r="F78" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G78" s="8" t="inlineStr">
@@ -11370,7 +11370,7 @@
       </c>
       <c r="F79" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G79" s="8" t="inlineStr">
@@ -11413,7 +11413,7 @@
       </c>
       <c r="F80" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G80" s="8" t="inlineStr">
@@ -11456,7 +11456,7 @@
       </c>
       <c r="F81" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G81" s="8" t="inlineStr">
@@ -11499,7 +11499,7 @@
       </c>
       <c r="F82" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G82" s="8" t="inlineStr">
@@ -11542,7 +11542,7 @@
       </c>
       <c r="F83" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G83" s="8" t="inlineStr">
@@ -11585,7 +11585,7 @@
       </c>
       <c r="F84" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G84" s="8" t="inlineStr">
@@ -11628,7 +11628,7 @@
       </c>
       <c r="F85" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G85" s="8" t="inlineStr">
@@ -11671,7 +11671,7 @@
       </c>
       <c r="F86" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G86" s="8" t="inlineStr">
@@ -11714,7 +11714,7 @@
       </c>
       <c r="F87" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G87" s="8" t="inlineStr">
@@ -11800,7 +11800,7 @@
       </c>
       <c r="F89" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G89" s="8" t="inlineStr">
@@ -11843,7 +11843,7 @@
       </c>
       <c r="F90" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G90" s="8" t="inlineStr">
@@ -11886,7 +11886,7 @@
       </c>
       <c r="F91" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G91" s="8" t="inlineStr">
@@ -11929,7 +11929,7 @@
       </c>
       <c r="F92" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G92" s="8" t="inlineStr">
@@ -11972,7 +11972,7 @@
       </c>
       <c r="F93" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G93" s="8" t="inlineStr">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="F94" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G94" s="8" t="inlineStr">
@@ -12144,7 +12144,7 @@
       </c>
       <c r="F97" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G97" s="8" t="inlineStr">
@@ -12187,7 +12187,7 @@
       </c>
       <c r="F98" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G98" s="8" t="inlineStr">
@@ -12230,7 +12230,7 @@
       </c>
       <c r="F99" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G99" s="8" t="inlineStr">
@@ -12316,7 +12316,7 @@
       </c>
       <c r="F101" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G101" s="8" t="inlineStr">
@@ -12359,7 +12359,7 @@
       </c>
       <c r="F102" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G102" s="8" t="inlineStr">
@@ -12402,7 +12402,7 @@
       </c>
       <c r="F103" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G103" s="8" t="inlineStr">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="F104" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G104" s="8" t="inlineStr">
@@ -12488,7 +12488,7 @@
       </c>
       <c r="F105" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G105" s="8" t="inlineStr">
@@ -12531,7 +12531,7 @@
       </c>
       <c r="F106" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G106" s="8" t="inlineStr">
@@ -12574,7 +12574,7 @@
       </c>
       <c r="F107" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G107" s="8" t="inlineStr">
@@ -12617,7 +12617,7 @@
       </c>
       <c r="F108" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G108" s="8" t="inlineStr">
@@ -12703,7 +12703,7 @@
       </c>
       <c r="F110" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G110" s="8" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="F111" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G111" s="8" t="inlineStr">
@@ -12789,7 +12789,7 @@
       </c>
       <c r="F112" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G112" s="8" t="inlineStr">
@@ -12832,7 +12832,7 @@
       </c>
       <c r="F113" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G113" s="8" t="inlineStr">
@@ -12918,7 +12918,7 @@
       </c>
       <c r="F115" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G115" s="8" t="inlineStr">
@@ -12961,7 +12961,7 @@
       </c>
       <c r="F116" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G116" s="8" t="inlineStr">
@@ -13004,7 +13004,7 @@
       </c>
       <c r="F117" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G117" s="8" t="inlineStr">
@@ -13047,7 +13047,7 @@
       </c>
       <c r="F118" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G118" s="8" t="inlineStr">
@@ -13090,7 +13090,7 @@
       </c>
       <c r="F119" s="8" t="inlineStr">
         <is>
-          <t>Apathetic</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G119" s="8" t="inlineStr">
@@ -13133,7 +13133,7 @@
       </c>
       <c r="F120" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G120" s="8" t="inlineStr">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="F121" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G121" s="8" t="inlineStr">
@@ -13219,7 +13219,7 @@
       </c>
       <c r="F122" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G122" s="8" t="inlineStr">
@@ -13262,7 +13262,7 @@
       </c>
       <c r="F123" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G123" s="8" t="inlineStr">
@@ -13305,7 +13305,7 @@
       </c>
       <c r="F124" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G124" s="8" t="inlineStr">
@@ -13348,7 +13348,7 @@
       </c>
       <c r="F125" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G125" s="8" t="inlineStr">
@@ -13391,7 +13391,7 @@
       </c>
       <c r="F126" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G126" s="8" t="inlineStr">
@@ -13434,7 +13434,7 @@
       </c>
       <c r="F127" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G127" s="8" t="inlineStr">
@@ -13477,7 +13477,7 @@
       </c>
       <c r="F128" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G128" s="8" t="inlineStr">
@@ -13520,7 +13520,7 @@
       </c>
       <c r="F129" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G129" s="8" t="inlineStr">
@@ -13563,7 +13563,7 @@
       </c>
       <c r="F130" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G130" s="8" t="inlineStr">
@@ -13606,7 +13606,7 @@
       </c>
       <c r="F131" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G131" s="8" t="inlineStr">
@@ -13649,7 +13649,7 @@
       </c>
       <c r="F132" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G132" s="8" t="inlineStr">
@@ -13692,7 +13692,7 @@
       </c>
       <c r="F133" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G133" s="8" t="inlineStr">
@@ -13735,7 +13735,7 @@
       </c>
       <c r="F134" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G134" s="8" t="inlineStr">
@@ -13778,7 +13778,7 @@
       </c>
       <c r="F135" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G135" s="8" t="inlineStr">
@@ -13821,7 +13821,7 @@
       </c>
       <c r="F136" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G136" s="8" t="inlineStr">
@@ -13864,7 +13864,7 @@
       </c>
       <c r="F137" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G137" s="8" t="inlineStr">
@@ -13907,7 +13907,7 @@
       </c>
       <c r="F138" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G138" s="8" t="inlineStr">
@@ -14036,7 +14036,7 @@
       </c>
       <c r="F141" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G141" s="8" t="inlineStr">
@@ -14122,7 +14122,7 @@
       </c>
       <c r="F143" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G143" s="8" t="inlineStr">
@@ -14165,7 +14165,7 @@
       </c>
       <c r="F144" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G144" s="8" t="inlineStr">
@@ -14208,7 +14208,7 @@
       </c>
       <c r="F145" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G145" s="8" t="inlineStr">
@@ -14251,7 +14251,7 @@
       </c>
       <c r="F146" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G146" s="8" t="inlineStr">
@@ -14294,7 +14294,7 @@
       </c>
       <c r="F147" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G147" s="8" t="inlineStr">
@@ -14337,7 +14337,7 @@
       </c>
       <c r="F148" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G148" s="8" t="inlineStr">
@@ -14380,7 +14380,7 @@
       </c>
       <c r="F149" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G149" s="8" t="inlineStr">
@@ -14423,7 +14423,7 @@
       </c>
       <c r="F150" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G150" s="8" t="inlineStr">
@@ -14466,7 +14466,7 @@
       </c>
       <c r="F151" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G151" s="8" t="inlineStr">
@@ -14509,7 +14509,7 @@
       </c>
       <c r="F152" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G152" s="8" t="inlineStr">
@@ -14552,7 +14552,7 @@
       </c>
       <c r="F153" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G153" s="8" t="inlineStr">
@@ -14595,7 +14595,7 @@
       </c>
       <c r="F154" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G154" s="8" t="inlineStr">
@@ -14638,7 +14638,7 @@
       </c>
       <c r="F155" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G155" s="8" t="inlineStr">
@@ -14681,7 +14681,7 @@
       </c>
       <c r="F156" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G156" s="8" t="inlineStr">
@@ -14724,7 +14724,7 @@
       </c>
       <c r="F157" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G157" s="8" t="inlineStr">
@@ -14767,7 +14767,7 @@
       </c>
       <c r="F158" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G158" s="8" t="inlineStr">
@@ -14810,7 +14810,7 @@
       </c>
       <c r="F159" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G159" s="8" t="inlineStr">
@@ -14853,7 +14853,7 @@
       </c>
       <c r="F160" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G160" s="8" t="inlineStr">
@@ -14896,7 +14896,7 @@
       </c>
       <c r="F161" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G161" s="8" t="inlineStr">
@@ -14939,7 +14939,7 @@
       </c>
       <c r="F162" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G162" s="8" t="inlineStr">
@@ -14982,7 +14982,7 @@
       </c>
       <c r="F163" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G163" s="8" t="inlineStr">
@@ -15025,7 +15025,7 @@
       </c>
       <c r="F164" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G164" s="8" t="inlineStr">
@@ -15068,7 +15068,7 @@
       </c>
       <c r="F165" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G165" s="8" t="inlineStr">
@@ -15111,7 +15111,7 @@
       </c>
       <c r="F166" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G166" s="8" t="inlineStr">
@@ -15154,7 +15154,7 @@
       </c>
       <c r="F167" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G167" s="8" t="inlineStr">
@@ -15197,7 +15197,7 @@
       </c>
       <c r="F168" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G168" s="8" t="inlineStr">
@@ -15240,7 +15240,7 @@
       </c>
       <c r="F169" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G169" s="8" t="inlineStr">
@@ -15283,7 +15283,7 @@
       </c>
       <c r="F170" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G170" s="8" t="inlineStr">
@@ -15326,7 +15326,7 @@
       </c>
       <c r="F171" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G171" s="8" t="inlineStr">
@@ -15369,7 +15369,7 @@
       </c>
       <c r="F172" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G172" s="8" t="inlineStr">
@@ -15412,7 +15412,7 @@
       </c>
       <c r="F173" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G173" s="8" t="inlineStr">
@@ -15455,7 +15455,7 @@
       </c>
       <c r="F174" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G174" s="8" t="inlineStr">
@@ -15498,7 +15498,7 @@
       </c>
       <c r="F175" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G175" s="8" t="inlineStr">
@@ -15541,7 +15541,7 @@
       </c>
       <c r="F176" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G176" s="8" t="inlineStr">
@@ -15584,7 +15584,7 @@
       </c>
       <c r="F177" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G177" s="8" t="inlineStr">
@@ -15627,7 +15627,7 @@
       </c>
       <c r="F178" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G178" s="8" t="inlineStr">
@@ -15670,7 +15670,7 @@
       </c>
       <c r="F179" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G179" s="8" t="inlineStr">
@@ -15713,7 +15713,7 @@
       </c>
       <c r="F180" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G180" s="8" t="inlineStr">
@@ -15756,7 +15756,7 @@
       </c>
       <c r="F181" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Apathetic</t>
         </is>
       </c>
       <c r="G181" s="8" t="inlineStr">
@@ -15799,7 +15799,7 @@
       </c>
       <c r="F182" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Attracted</t>
         </is>
       </c>
       <c r="G182" s="8" t="inlineStr">
@@ -15842,7 +15842,7 @@
       </c>
       <c r="F183" s="8" t="inlineStr">
         <is>
-          <t>Unattracted</t>
+          <t>Impassioned</t>
         </is>
       </c>
       <c r="G183" s="8" t="inlineStr">

</xml_diff>